<commit_message>
Added legend and highlight mpp lab1
</commit_message>
<xml_diff>
--- a/Labs/renewable Lab1.xlsx
+++ b/Labs/renewable Lab1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2019\Renewable Energy Systems\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC34BCAE-0F2D-42F6-B7D2-930FF553B471}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D74374-5135-4BDB-AC14-A3E9B02B809B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -293,6 +293,130 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:marker>
+              <c:symbol val="x"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-F5A4-4FDB-B5CC-71294AF167C4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP:</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{0B71F88D-8F61-43DC-BA89-C5ABDF10AF18}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> A</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F5A4-4FDB-B5CC-71294AF167C4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$15</c:f>
@@ -807,6 +931,106 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP:</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{86A0BBE4-D750-4A24-8001-F7199D749B93}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> A</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-D8E6-4B07-9B39-5D46712AA366}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$20:$A$32</c:f>
@@ -1318,6 +1542,102 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP: </a:t>
+                    </a:r>
+                    <a:fld id="{926B6D29-68DD-4A29-913D-706333AF9D4A}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> A </a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-E383-416C-A47F-D9CE4AADBC90}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$37:$A$49</c:f>
@@ -1824,6 +2144,154 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:noAutofit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP:</a:t>
+                    </a:r>
+                    <a:fld id="{3D605652-9BA2-4CBC-88EC-2F9257EDBBB2}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr>
+                        <a:defRPr/>
+                      </a:pPr>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> W</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:noAutofit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.26621992113877258"/>
+                      <c:h val="7.7753759456087729E-2"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-DDBC-447F-A0E3-3365E6114264}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$15</c:f>
@@ -2335,6 +2803,112 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP:</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{CB297963-7A1B-4E2A-A40A-1B50BE6820FF}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> W</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.30948549486892274"/>
+                      <c:h val="0.1143071047107133"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-4C66-49D2-AFB8-BBF509F84C5F}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$20:$A$32</c:f>
@@ -2846,6 +3420,112 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>MPP:</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{35387FB0-5453-4EF5-9C82-F3E910BD1726}" type="YVALUE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[Y VALUE]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t> W</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="t"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.34576095635387449"/>
+                      <c:h val="0.11430714591328676"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-0CCE-4C79-8145-3441F8DFE686}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$37:$A$49</c:f>
@@ -7083,8 +7763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="103" workbookViewId="0">
+      <selection activeCell="X32" sqref="X32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
finalising graph lab 1
</commit_message>
<xml_diff>
--- a/Labs/renewable Lab1.xlsx
+++ b/Labs/renewable Lab1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Spring 2019\Renewable Energy Systems\Labs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D74374-5135-4BDB-AC14-A3E9B02B809B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7E03F3-2667-40A4-A7C7-BDA2F3F7EA96}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2223,12 +2223,15 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.26621992113877258"/>
-                      <c:h val="7.7753759456087729E-2"/>
-                    </c:manualLayout>
-                  </c15:layout>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:prstGeom prst="rect">
+                      <a:avLst/>
+                    </a:prstGeom>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                  </c15:spPr>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -2840,12 +2843,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.30948549486892274"/>
-                      <c:h val="0.1143071047107133"/>
-                    </c:manualLayout>
-                  </c15:layout>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="0"/>
                 </c:ext>
@@ -3459,8 +3456,8 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
-                      <c:w val="0.34576095635387449"/>
-                      <c:h val="0.11430714591328676"/>
+                      <c:w val="0.34975000000000001"/>
+                      <c:h val="0.11395041818842985"/>
                     </c:manualLayout>
                   </c15:layout>
                   <c15:dlblFieldTable/>
@@ -7763,8 +7760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="103" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>